<commit_message>
Modification des erreurs repérées
</commit_message>
<xml_diff>
--- a/Projet_4_La_chouette_agence/Modèle-audit-SEO.xlsx
+++ b/Projet_4_La_chouette_agence/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzzammilpeerboccus/Documents/ProjetOpenClassrooms/Projet_4_La_chouette_agence/Projet_4_La_chouette_agence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5D44FE-04AF-234E-B962-DF94382B29E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E788C4-7366-AA40-A9E1-F5218921FDC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28780" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28780" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -198,18 +198,6 @@
     <t>Dissocier les 2 blocs et mettre une marge entre les 2</t>
   </si>
   <si>
-    <t>Utilisation excessive de sélecteurs (class=)</t>
-  </si>
-  <si>
-    <t>Il y a beaucoup trop de sélecteurs pour un seul bloc afin de définir seulement quelques valeurs</t>
-  </si>
-  <si>
-    <t>Il faut mettre le minimum de sélecteurs pour définir les propriétés et les valeurs d'un bloc</t>
-  </si>
-  <si>
-    <t>Réduire le nombre de sélecteur en mettant les valeurs dans un seul sélecteur</t>
-  </si>
-  <si>
     <t>Des textes trop long contenant aucun mot clé</t>
   </si>
   <si>
@@ -234,9 +222,6 @@
     <t xml:space="preserve">Mettre les bons liens des reseaux sociaux </t>
   </si>
   <si>
-    <t>Attribut ALT trop long</t>
-  </si>
-  <si>
     <t>L'attribut ALT des images est beaucoup trop long et ne représente pas l'image ce qui ne respecte pas les normes WCAG</t>
   </si>
   <si>
@@ -249,9 +234,6 @@
     <t>Sur certaines parties du site il y a des problèmes de contrastes couleurs ce qui restreint l'accessibilité et la visibilité</t>
   </si>
   <si>
-    <t>Le site non responsive</t>
-  </si>
-  <si>
     <t>Un site doit impérativement être responsive afin de s'adapter à toute sorte d'écran et favoriser donc un meilleur SEO</t>
   </si>
   <si>
@@ -261,27 +243,6 @@
     <t>Réaliser le responsive du site</t>
   </si>
   <si>
-    <t>Le même CSS pour les 2 pages</t>
-  </si>
-  <si>
-    <t>Les 2 pages HTML possède le même ce qui n'est pas bon pour le référencement naturel et l'organisation du code</t>
-  </si>
-  <si>
-    <t>Dissocier le CSS de chaque pages HTML</t>
-  </si>
-  <si>
-    <t>Plusieurs sélecteurs dans le CSS se répetent inutilement ce qui engendre une mauvaise structure et donc réduit le SEO</t>
-  </si>
-  <si>
-    <t>Il faut faire en sorte de minifier au maximum son code afin d'avoir une bonne structure et augmenter le SEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minifier au mieux le code </t>
-  </si>
-  <si>
-    <t>Répétition de plusieurs sélecteur dans le CSS</t>
-  </si>
-  <si>
     <t>Il y 3 fois la possibilité de contact, un lien vers l'accueil dans l'accueil et même problème page 2 ce qui n'est pas favorable aux normes SEO</t>
   </si>
   <si>
@@ -291,20 +252,59 @@
     <t>Le site n'est pas structuré avec des balises sémantiques ce qui empêche les personnes utilisant des technologie d'assistance de s'y retrouver et la force du référencement naturel</t>
   </si>
   <si>
-    <t xml:space="preserve">Il faut avoir un code organisé pour un bon référencement naturel donc préférable d'avoir un CSS pour chaque pages </t>
-  </si>
-  <si>
     <t>Il faut toujours utiliser des balises sémantiques afin de donner une structure à son code et différencier les zones</t>
   </si>
   <si>
     <t>Ajouter au code les balises sémantiques pour une meilleure organisation</t>
+  </si>
+  <si>
+    <t>Attribut ALT non conforme</t>
+  </si>
+  <si>
+    <t>Le site mal responsive</t>
+  </si>
+  <si>
+    <t>Format image trop volumineux</t>
+  </si>
+  <si>
+    <t>Les images présents sur le site sont beaucoup trop lourde et ralentit le site</t>
+  </si>
+  <si>
+    <t>Il faut réduire le volume des images afin d'augmenter les performances et la vitesse du site</t>
+  </si>
+  <si>
+    <t>Il faut conseiller d'avoir des images en faible résolution afin de permettre au site d'avoir fluide</t>
+  </si>
+  <si>
+    <t>Il faut toujours avoir une meta description afin d'avoir un référencement optimal et décrire logiquement le site</t>
+  </si>
+  <si>
+    <t>Ajouter une meta description qui résume de manière concis le site</t>
+  </si>
+  <si>
+    <t>Il y a des icones qui sont pré-enregistrés dans un fichier CSS mais qui ne sont pas utilisé dans le site</t>
+  </si>
+  <si>
+    <t>Il faut mettre uniquement dans son CSS ou HTML ce qui sera uniquement ajouté au site ou modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effacer ces icons qui ralentisent le site </t>
+  </si>
+  <si>
+    <t>Et-icon non utile pour le site web</t>
+  </si>
+  <si>
+    <t>Meta description non renseigné</t>
+  </si>
+  <si>
+    <t>Il n'y a aucun meta description qui résume l'utilité du site et donc n'optimise pas le référencement naturel et ne permet pas de décrire le site aux personnes utilisant une assistance vocale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,13 +326,27 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -369,17 +383,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,19 +625,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B6095" sqref="B6095"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="138" customWidth="1"/>
-    <col min="4" max="4" width="91.42578125" customWidth="1"/>
-    <col min="5" max="5" width="57.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="26" width="10.5703125" customWidth="1"/>
   </cols>
@@ -652,347 +682,347 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>31</v>
+      <c r="D19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="20" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>35</v>
+      <c r="B20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>38</v>
+    <row r="21" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1968,9 +1998,6 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Amélioration partie 1 du site
</commit_message>
<xml_diff>
--- a/Projet_4_La_chouette_agence/Modèle-audit-SEO.xlsx
+++ b/Projet_4_La_chouette_agence/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzzammilpeerboccus/Documents/ProjetOpenClassrooms/Projet_4_La_chouette_agence/Projet_4_La_chouette_agence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E788C4-7366-AA40-A9E1-F5218921FDC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0740D446-E7D6-9447-AE17-65AAE48A611A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28780" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>Mots clés dans le HTML</t>
   </si>
   <si>
-    <t>Des paragraphes sont des images ce qui empêche les mal voyannt de traduire la page</t>
-  </si>
-  <si>
     <t>Le titre est un simple "." ce qui ne donne pas de nom à la page et emêche sa traduction</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>Il n'y a aucun meta description qui résume l'utilité du site et donc n'optimise pas le référencement naturel et ne permet pas de décrire le site aux personnes utilisant une assistance vocale</t>
+  </si>
+  <si>
+    <t>Des paragraphes sont des images ce qui empêche les mal voyant de traduire la page</t>
   </si>
 </sst>
 </file>
@@ -350,7 +350,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,6 +361,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -383,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -408,6 +414,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -627,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6095" sqref="B6095"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -682,20 +710,20 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -707,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>11</v>
@@ -716,21 +744,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:26" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="C4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>17</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -738,84 +766,84 @@
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:26" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>28</v>
       </c>
+      <c r="C7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:26" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -823,16 +851,16 @@
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -840,33 +868,33 @@
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:26" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -874,16 +902,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -891,33 +919,33 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="15" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="1:26" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -925,16 +953,16 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -942,16 +970,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -959,33 +987,33 @@
         <v>6</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>74</v>
-      </c>
     </row>
-    <row r="19" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:5" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -993,16 +1021,16 @@
         <v>13</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1010,16 +1038,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="D21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Amélioration visuel du site
</commit_message>
<xml_diff>
--- a/Projet_4_La_chouette_agence/Modèle-audit-SEO.xlsx
+++ b/Projet_4_La_chouette_agence/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzzammilpeerboccus/Documents/ProjetOpenClassrooms/Projet_4_La_chouette_agence/Projet_4_La_chouette_agence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0740D446-E7D6-9447-AE17-65AAE48A611A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C5F91B-8B91-F34A-9C46-FC35A3DA37F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28780" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -727,20 +727,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:26" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -761,20 +761,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:26" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1033,20 +1033,20 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:5" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="14" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>